<commit_message>
Added pile-up correction feature to v20 code
</commit_message>
<xml_diff>
--- a/tables/grid_wire_channel_mapping.xlsx
+++ b/tables/grid_wire_channel_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbackis/Documents/mg_analysis_notebook/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA02C96-B007-974D-9485-8A3D47B52616}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBFE556-0886-D84A-A34C-AF5920E7FB48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19280" yWindow="-26140" windowWidth="16580" windowHeight="24860" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
+    <workbookView xWindow="6240" yWindow="600" windowWidth="16580" windowHeight="16480" xr2:uid="{AADEF4F3-1BBF-ED42-AB5A-7CEAA96F0BFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81663BE0-29B8-F646-A110-AC508EA7B182}">
   <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>